<commit_message>
Updated the Bug Metrics and Testcases
</commit_message>
<xml_diff>
--- a/Testing/Testcases.xlsx
+++ b/Testing/Testcases.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t6\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C5A29E-1CC6-4A33-8460-A3EB4148C8E5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A561E2-2625-4EFC-AEE7-A573A3845CD7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{E90EB661-BF25-40DF-8004-68D825EA22BE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Manual Testcase" sheetId="1" r:id="rId1"/>
-    <sheet name="Functional Index" sheetId="2" r:id="rId2"/>
+    <sheet name="Testcase Manual " sheetId="3" r:id="rId1"/>
+    <sheet name="Manual Testcase OLD" sheetId="1" r:id="rId2"/>
+    <sheet name="Functional Index" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="180">
   <si>
     <t>1.1, 1.2, 1.3</t>
   </si>
@@ -364,13 +365,463 @@
   </si>
   <si>
     <t>8.1.2.a, 8.1.2.b</t>
+  </si>
+  <si>
+    <t>The round 2 clearing logic is described below in more detail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Round 1 starts when the data.zip file is uploaded to the database through bootstrap. Round 1 ends when admin close round 1, and bidding results will be process and result reflected to students. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Admin clicks on end round, to close the round </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Closing a round prompts the admin for confirmation on closing a round, upon confirmation the round closes and round 2 begins.  </t>
+  </si>
+  <si>
+    <t>Input student id and password base on sample data uploaded and validated to database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fail, display incorrect User ID or Password </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Userid: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">amy.ng.2009
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> qwerty128</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Userid:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Password:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> qwerty128</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Userid:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Password: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Userid:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> test123
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Password: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test123</t>
+    </r>
+  </si>
+  <si>
+    <t>Admin to upload data.zip file via bootstrap to Database base on the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input various data files, some will contain with discrepancy for test purpose </t>
+  </si>
+  <si>
+    <t>Input data.zip file without Mandatory file, removal of course.csv</t>
+  </si>
+  <si>
+    <t>Output error to user that mandatory csv file is missing and requires reupload with mandatory file.</t>
+  </si>
+  <si>
+    <t>System output empty blank space</t>
+  </si>
+  <si>
+    <t>Input data file with extra csv file</t>
+  </si>
+  <si>
+    <t>Input given sample data file</t>
+  </si>
+  <si>
+    <t>exam date</t>
+  </si>
+  <si>
+    <t>Row 3</t>
+  </si>
+  <si>
+    <t>Alphanumeric exam date</t>
+  </si>
+  <si>
+    <t>Row 4</t>
+  </si>
+  <si>
+    <t>Date with space</t>
+  </si>
+  <si>
+    <t>Row 5</t>
+  </si>
+  <si>
+    <t>Date with extra numbers</t>
+  </si>
+  <si>
+    <t>Row 6</t>
+  </si>
+  <si>
+    <t>Incorrect Exam start 12.01</t>
+  </si>
+  <si>
+    <t>exam start</t>
+  </si>
+  <si>
+    <t>Row 7</t>
+  </si>
+  <si>
+    <t>Delete exam start</t>
+  </si>
+  <si>
+    <t>Row 8</t>
+  </si>
+  <si>
+    <t>Alphanumeric exam starts</t>
+  </si>
+  <si>
+    <t>Row 9</t>
+  </si>
+  <si>
+    <t>Edit exam starts value and re-edit back to normal</t>
+  </si>
+  <si>
+    <t>Row 10</t>
+  </si>
+  <si>
+    <t>Exam ends with less than given end time</t>
+  </si>
+  <si>
+    <t>exam end</t>
+  </si>
+  <si>
+    <t>Row 11</t>
+  </si>
+  <si>
+    <t>Exam ends with one of designated time with value greater assigned value</t>
+  </si>
+  <si>
+    <t>Row 12</t>
+  </si>
+  <si>
+    <t>Exam ends with one of designated time with value lower assigned value</t>
+  </si>
+  <si>
+    <t>Row 13</t>
+  </si>
+  <si>
+    <t>Delete exam end</t>
+  </si>
+  <si>
+    <t>Row 14</t>
+  </si>
+  <si>
+    <t>title more than 100 characters.</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Row 15</t>
+  </si>
+  <si>
+    <t>Delete title</t>
+  </si>
+  <si>
+    <t>Row 16</t>
+  </si>
+  <si>
+    <t>Delete description</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Row 17</t>
+  </si>
+  <si>
+    <t>description more than 100 characters.</t>
+  </si>
+  <si>
+    <t>Row 18</t>
+  </si>
+  <si>
+    <t>Delete course</t>
+  </si>
+  <si>
+    <t>course</t>
+  </si>
+  <si>
+    <t>Row 19</t>
+  </si>
+  <si>
+    <t>Edit course</t>
+  </si>
+  <si>
+    <t>Row 20</t>
+  </si>
+  <si>
+    <t>Edit school</t>
+  </si>
+  <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Row 22</t>
+  </si>
+  <si>
+    <t>Delete School</t>
+  </si>
+  <si>
+    <t>exam date Column</t>
+  </si>
+  <si>
+    <t>Input data.zip file - Course.csv Row 2 - Exam Date Column - Delete exam date</t>
+  </si>
+  <si>
+    <t>Fail and output to error display message to user</t>
+  </si>
+  <si>
+    <t>Input data.zip file - Course.csv - Row 2 - Exam Date Column (Blank Exam Date)</t>
+  </si>
+  <si>
+    <t>Input data.zip file - Course.csv - Row 3 - Exam Date Column (Alphanumeric Exam Date)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.) PHP Error - Notice: Undefined variable: result in C:\Users\User\Documents\GitHub\project-g4t6\app\include\StudentDAO.php on line 61</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2.) Fail, display incorrect User ID or Password</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PHP Error - Warning: checkdate() expects parameter 3 to be integer, string given in C:\Users\User\Documents\GitHub\project-g4t6\app\include\bootstrapValidate.php on line 22 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A non well formed numeric value encountered in C:\Users\User\Documents\GitHub\project-g4t6\app\include\bootstrapValidate.php on line 22</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PHP Error - Fatal error: Uncaught PDOException: SQLSTATE[22007]: Invalid datetime format: 1292 Incorrect date value: '201a1118' for column 'examdate' at row 1 in C:\Users\User\Documents\GitHub\project-g4t6\app\include\CourseDAO.php on line 23 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> PDOException: SQLSTATE[22007]: Invalid datetime format: 1292 Incorrect date value: '201a1118' for column 'examdate' at row 1 in C:\Users\User\Documents\GitHub\project-g4t6\app\include\CourseDAO.php on line 23</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,8 +863,17 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,8 +898,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -497,11 +963,177 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -542,50 +1174,158 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,11 +1640,1030 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4A64FB-D5C5-440E-AB26-01D6449FC916}">
+  <dimension ref="A1:I66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="47.77734375" customWidth="1"/>
+    <col min="4" max="4" width="80.88671875" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" customWidth="1"/>
+    <col min="6" max="6" width="75.5546875" customWidth="1"/>
+    <col min="7" max="7" width="42.109375" customWidth="1"/>
+    <col min="8" max="8" width="148.109375" customWidth="1"/>
+    <col min="9" max="9" width="23.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:9" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36">
+        <v>1</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="37"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="34"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="37"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="I5" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="37"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="34"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="37"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="37"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="34"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="G9" s="45" t="s">
+        <v>115</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="49">
+        <v>7</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
+      <c r="E12" s="51"/>
+      <c r="F12" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="H14" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="H15" s="31" t="s">
+        <v>179</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="19"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="19"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="19"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="19"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="19"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="19"/>
+    </row>
+    <row r="29" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="I29" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="3"/>
+      <c r="B30" s="16"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="H30" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="G31" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I31" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G32" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="H32" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="I32" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="G33" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="H33" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="26" t="s">
+        <v>137</v>
+      </c>
+      <c r="G34" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="H34" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="3"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="G36" s="27" t="s">
+        <v>142</v>
+      </c>
+      <c r="H36" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="I36" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="17"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H37" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="3"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="17"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="H38" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="I38" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="H39" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="I39" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="H40" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="I40" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="G41" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="H41" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="I41" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="17"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="I42" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="H43" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I43" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="3"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="17"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="H44" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I44" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="17"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="G45" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="H45" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="I45" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="3"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="G46" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H46" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="I46" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="18"/>
+      <c r="F47" s="26" t="s">
+        <v>165</v>
+      </c>
+      <c r="G47" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H47" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="I47" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="3"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="17"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="G48" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="H48" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="I48" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="17"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="H49" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="I49" s="27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="17"/>
+      <c r="D50" s="18"/>
+      <c r="E50" s="18"/>
+      <c r="F50" s="18"/>
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="19"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="3"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="19"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="3"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="17"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18"/>
+      <c r="F52" s="18"/>
+      <c r="G52" s="18"/>
+      <c r="H52" s="18"/>
+      <c r="I52" s="19"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="3"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="19"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="3"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="18"/>
+      <c r="I54" s="19"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="3"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="17"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="19"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="3"/>
+      <c r="B56" s="16"/>
+      <c r="C56" s="17"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="19"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="3"/>
+      <c r="B57" s="16"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="19"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="3"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="19"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="3"/>
+      <c r="B59" s="16"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="19"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="3"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="19"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="3"/>
+      <c r="B61" s="16"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="19"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A62" s="3"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="18"/>
+      <c r="I62" s="19"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="3"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+      <c r="H63" s="18"/>
+      <c r="I63" s="19"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A64" s="3"/>
+      <c r="B64" s="16"/>
+      <c r="C64" s="17"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="19"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="D11:D16"/>
+    <mergeCell ref="E11:E16"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="D3:D10"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5331B76C-43B6-4CD9-94DC-A6FA54967D91}">
   <dimension ref="B1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -954,757 +2713,785 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="25">
+      <c r="B3" s="49">
         <v>1</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="63" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="25"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="27"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="66"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="63"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="22"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="27"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="66"/>
+      <c r="K5" s="61"/>
+      <c r="L5" s="63"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="22"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="27"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="66"/>
+      <c r="K6" s="61"/>
+      <c r="L6" s="63"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="22"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="27"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="66"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="63"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="25"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="22"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="27"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="66"/>
+      <c r="K8" s="61"/>
+      <c r="L8" s="63"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="16">
+      <c r="B9" s="59">
         <v>2</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="I9" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="18" t="s">
+      <c r="K9" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="64" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="16"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="17"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="30"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="56"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="64"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="17"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="30"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="56"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="64"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="16"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="17"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="30"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="56"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="64"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="16"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="17"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="30"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="56"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="64"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="16"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="17"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="30"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
+      <c r="I14" s="56"/>
+      <c r="K14" s="61"/>
+      <c r="L14" s="64"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="16">
+      <c r="B15" s="59">
         <v>3</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="60" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="G15" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="16" t="s">
+      <c r="H15" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="18"/>
+      <c r="K15" s="61"/>
       <c r="L15" s="15"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="16"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="17"/>
-      <c r="K16" s="18"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="57"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="56"/>
+      <c r="K16" s="61"/>
       <c r="L16" s="15"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="16"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="17"/>
-      <c r="K17" s="18"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="56"/>
+      <c r="K17" s="61"/>
       <c r="L17" s="15"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="16"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="17"/>
-      <c r="K18" s="18"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="56"/>
+      <c r="K18" s="61"/>
       <c r="L18" s="15"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="16"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="17"/>
-      <c r="K19" s="18"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="56"/>
+      <c r="K19" s="61"/>
       <c r="L19" s="15"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="16"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="17"/>
-      <c r="K20" s="18"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="56"/>
+      <c r="K20" s="61"/>
       <c r="L20" s="15"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="16">
+      <c r="B21" s="59">
         <v>4</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="60" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="17" t="s">
+      <c r="I21" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="K21" s="18"/>
+      <c r="K21" s="61"/>
       <c r="L21" s="15"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="16"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
-      <c r="K22" s="18"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="56"/>
+      <c r="K22" s="61"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="16"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="17"/>
-      <c r="K23" s="18"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="56"/>
+      <c r="K23" s="61"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="16"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="17"/>
-      <c r="K24" s="18"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="57"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="56"/>
+      <c r="K24" s="61"/>
       <c r="L24" s="15"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="16"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="17"/>
-      <c r="K25" s="18"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="56"/>
+      <c r="K25" s="61"/>
       <c r="L25" s="15"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="16"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="17"/>
-      <c r="K26" s="18"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="60"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="56"/>
+      <c r="K26" s="61"/>
       <c r="L26" s="15"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="16">
+      <c r="B27" s="59">
         <v>5</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="60">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="57" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G27" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H27" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="K27" s="28" t="s">
+      <c r="K27" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="L27" s="27"/>
+      <c r="L27" s="63"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="17"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="27"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="60"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="57"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="56"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="63"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="16"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="17"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="27"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="56"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="63"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="16"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="17"/>
-      <c r="K30" s="28"/>
-      <c r="L30" s="27"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="57"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="57"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="56"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="63"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="16"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="17"/>
-      <c r="K31" s="28"/>
-      <c r="L31" s="27"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="57"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="57"/>
+      <c r="H31" s="57"/>
+      <c r="I31" s="56"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="63"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="16"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="17"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="27"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="57"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="57"/>
+      <c r="H32" s="57"/>
+      <c r="I32" s="56"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="63"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="16">
+      <c r="B33" s="59">
         <v>6</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="60" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="57" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="57" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="16" t="s">
+      <c r="H33" s="59" t="s">
         <v>92</v>
       </c>
-      <c r="I33" s="17" t="s">
+      <c r="I33" s="56" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="16"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="17"/>
+      <c r="B34" s="59"/>
+      <c r="C34" s="60"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="57"/>
+      <c r="F34" s="57"/>
+      <c r="G34" s="57"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="56"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="16"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="17"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="57"/>
+      <c r="E35" s="57"/>
+      <c r="F35" s="57"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="56"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="16"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="17"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="60"/>
+      <c r="D36" s="57"/>
+      <c r="E36" s="57"/>
+      <c r="F36" s="57"/>
+      <c r="G36" s="57"/>
+      <c r="H36" s="59"/>
+      <c r="I36" s="56"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="16"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="17"/>
+      <c r="B37" s="59"/>
+      <c r="C37" s="60"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="57"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="57"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="56"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="16"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="17"/>
+      <c r="B38" s="59"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
+      <c r="G38" s="57"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="56"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="16">
+      <c r="B39" s="59">
         <v>7</v>
       </c>
-      <c r="C39" s="19" t="s">
+      <c r="C39" s="60" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G39" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="H39" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="I39" s="17" t="s">
+      <c r="I39" s="56" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="16"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="17"/>
+      <c r="B40" s="59"/>
+      <c r="C40" s="60"/>
+      <c r="D40" s="57"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+      <c r="H40" s="57"/>
+      <c r="I40" s="56"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="16"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="17"/>
+      <c r="B41" s="59"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+      <c r="H41" s="57"/>
+      <c r="I41" s="56"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="16"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="17"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="57"/>
+      <c r="E42" s="57"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="56"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="16"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="17"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="57"/>
+      <c r="E43" s="57"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="56"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="16"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="17"/>
+      <c r="B44" s="59"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="57"/>
+      <c r="E44" s="57"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+      <c r="H44" s="57"/>
+      <c r="I44" s="56"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="29">
+      <c r="B45" s="59">
         <v>8</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="60" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
+      <c r="D45" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="F45" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="H45" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="I45" s="59" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="29"/>
-      <c r="C46" s="23"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
+      <c r="B46" s="59"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="58"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="29"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
+      <c r="B47" s="59"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="57"/>
+      <c r="E47" s="57"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="58"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="59"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="29"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
+      <c r="B48" s="59"/>
+      <c r="C48" s="60"/>
+      <c r="D48" s="57"/>
+      <c r="E48" s="57"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="58"/>
+      <c r="H48" s="59"/>
+      <c r="I48" s="59"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="29"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
+      <c r="B49" s="59"/>
+      <c r="C49" s="60"/>
+      <c r="D49" s="57"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="59"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="29"/>
-      <c r="C50" s="23"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24"/>
-      <c r="I50" s="24"/>
+      <c r="B50" s="59"/>
+      <c r="C50" s="60"/>
+      <c r="D50" s="57"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="59"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="29">
+      <c r="B51" s="54">
         <v>8</v>
       </c>
-      <c r="C51" s="23" t="s">
+      <c r="C51" s="55" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="24"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="53"/>
+      <c r="H51" s="53"/>
+      <c r="I51" s="53"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="29"/>
-      <c r="C52" s="23"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="53"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="29"/>
-      <c r="C53" s="23"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
+      <c r="B53" s="54"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="53"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="53"/>
+      <c r="G53" s="53"/>
+      <c r="H53" s="53"/>
+      <c r="I53" s="53"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="29"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24"/>
+      <c r="B54" s="54"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="53"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="53"/>
+      <c r="G54" s="53"/>
+      <c r="H54" s="53"/>
+      <c r="I54" s="53"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="29"/>
-      <c r="C55" s="23"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
+      <c r="B55" s="54"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="53"/>
+      <c r="H55" s="53"/>
+      <c r="I55" s="53"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="29"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
+      <c r="B56" s="54"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="53"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="53"/>
+      <c r="G56" s="53"/>
+      <c r="H56" s="53"/>
+      <c r="I56" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="G51:G56"/>
-    <mergeCell ref="H51:H56"/>
-    <mergeCell ref="I51:I56"/>
-    <mergeCell ref="B51:B56"/>
-    <mergeCell ref="C51:C56"/>
-    <mergeCell ref="D51:D56"/>
-    <mergeCell ref="E51:E56"/>
-    <mergeCell ref="F51:F56"/>
-    <mergeCell ref="I39:I44"/>
-    <mergeCell ref="D45:D50"/>
-    <mergeCell ref="E45:E50"/>
-    <mergeCell ref="F45:F50"/>
-    <mergeCell ref="G45:G50"/>
-    <mergeCell ref="H45:H50"/>
-    <mergeCell ref="I45:I50"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="C45:C50"/>
-    <mergeCell ref="E39:E44"/>
-    <mergeCell ref="F39:F44"/>
+    <mergeCell ref="I21:I26"/>
+    <mergeCell ref="K15:K20"/>
+    <mergeCell ref="K21:K26"/>
+    <mergeCell ref="G15:G20"/>
+    <mergeCell ref="H15:H20"/>
+    <mergeCell ref="G21:G26"/>
+    <mergeCell ref="H21:H26"/>
+    <mergeCell ref="G3:G8"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="I3:I8"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="C39:C44"/>
+    <mergeCell ref="D33:D38"/>
+    <mergeCell ref="E33:E38"/>
+    <mergeCell ref="F33:F38"/>
+    <mergeCell ref="G33:G38"/>
+    <mergeCell ref="H33:H38"/>
+    <mergeCell ref="I33:I38"/>
+    <mergeCell ref="D39:D44"/>
+    <mergeCell ref="E27:E32"/>
+    <mergeCell ref="G9:G14"/>
+    <mergeCell ref="G39:G44"/>
+    <mergeCell ref="H39:H44"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="F3:F8"/>
+    <mergeCell ref="L27:L32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
     <mergeCell ref="K3:K8"/>
     <mergeCell ref="K27:K32"/>
     <mergeCell ref="L3:L8"/>
@@ -1721,65 +3508,49 @@
     <mergeCell ref="D9:D14"/>
     <mergeCell ref="E9:E14"/>
     <mergeCell ref="F9:F14"/>
-    <mergeCell ref="L27:L32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="G3:G8"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="I3:I8"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="C39:C44"/>
-    <mergeCell ref="D33:D38"/>
-    <mergeCell ref="E33:E38"/>
-    <mergeCell ref="F33:F38"/>
-    <mergeCell ref="G33:G38"/>
-    <mergeCell ref="H33:H38"/>
-    <mergeCell ref="I33:I38"/>
-    <mergeCell ref="D39:D44"/>
-    <mergeCell ref="E27:E32"/>
-    <mergeCell ref="G9:G14"/>
-    <mergeCell ref="G39:G44"/>
-    <mergeCell ref="H39:H44"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="C45:C50"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="F39:F44"/>
     <mergeCell ref="D15:D20"/>
     <mergeCell ref="E15:E20"/>
     <mergeCell ref="F15:F20"/>
-    <mergeCell ref="G15:G20"/>
-    <mergeCell ref="H15:H20"/>
     <mergeCell ref="B21:B26"/>
     <mergeCell ref="C21:C26"/>
     <mergeCell ref="D21:D26"/>
     <mergeCell ref="E21:E26"/>
     <mergeCell ref="F21:F26"/>
-    <mergeCell ref="G21:G26"/>
-    <mergeCell ref="H21:H26"/>
-    <mergeCell ref="I21:I26"/>
-    <mergeCell ref="K15:K20"/>
-    <mergeCell ref="K21:K26"/>
+    <mergeCell ref="I39:I44"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="E45:E50"/>
+    <mergeCell ref="F45:F50"/>
+    <mergeCell ref="G45:G50"/>
+    <mergeCell ref="H45:H50"/>
+    <mergeCell ref="I45:I50"/>
+    <mergeCell ref="G51:G56"/>
+    <mergeCell ref="H51:H56"/>
+    <mergeCell ref="I51:I56"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="C51:C56"/>
+    <mergeCell ref="D51:D56"/>
+    <mergeCell ref="E51:E56"/>
+    <mergeCell ref="F51:F56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE41C69-7513-44E6-A818-D455BC48C7D6}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2271,7 +4042,7 @@
         <v>59</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>52</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bootstrap change and Testcases
Updated Bootstrap with minor changes. More to come.

Updated Testcases for changes to correct test cases for improved bug testing
</commit_message>
<xml_diff>
--- a/Testing/Testcases.xlsx
+++ b/Testing/Testcases.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project-g4t6\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B087E1-B4AD-4414-A1F5-19B75516ABED}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6957959-F260-4C5B-BEE9-096434783AF8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E90EB661-BF25-40DF-8004-68D825EA22BE}"/>
+    <workbookView xWindow="17805" yWindow="5235" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="5" xr2:uid="{E90EB661-BF25-40DF-8004-68D825EA22BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Testcase Manual " sheetId="3" r:id="rId1"/>
     <sheet name="Course.csv" sheetId="4" r:id="rId2"/>
     <sheet name="Section.csv" sheetId="5" r:id="rId3"/>
-    <sheet name="Manual Testcase OLD" sheetId="1" r:id="rId4"/>
-    <sheet name="Functional Index" sheetId="2" r:id="rId5"/>
+    <sheet name="Student.csv" sheetId="6" r:id="rId4"/>
+    <sheet name="Prerequisite.csv" sheetId="7" r:id="rId5"/>
+    <sheet name="Bid.csv" sheetId="8" r:id="rId6"/>
+    <sheet name="Manual Testcase OLD" sheetId="1" r:id="rId7"/>
+    <sheet name="Functional Index" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="245">
   <si>
     <t>1.1, 1.2, 1.3</t>
   </si>
@@ -919,6 +922,100 @@
   </si>
   <si>
     <t xml:space="preserve">No start </t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School </t>
+  </si>
+  <si>
+    <t>Edollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Username exceeds 128 characters </t>
+  </si>
+  <si>
+    <t>Same user ID as 3</t>
+  </si>
+  <si>
+    <t>Same user ID as 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password exceeds 128 characters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name exceeds 100 characters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Negative e dollars </t>
+  </si>
+  <si>
+    <t xml:space="preserve">School doesn't exist </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blank </t>
+  </si>
+  <si>
+    <t>Same user ID as 20</t>
+  </si>
+  <si>
+    <t>Same user ID as 21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prerequisite </t>
+  </si>
+  <si>
+    <t>Course doesn't exist</t>
+  </si>
+  <si>
+    <t>Course and prerequisite are the same</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>UserID  not found in student.csv</t>
+  </si>
+  <si>
+    <t>Negative amount</t>
+  </si>
+  <si>
+    <t>Prerequisite required</t>
+  </si>
+  <si>
+    <t>Less than 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More than 2  decimal places </t>
+  </si>
+  <si>
+    <t>Section not found in section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Course not found in Course </t>
+  </si>
+  <si>
+    <t>Not from the correct school. Reject if Window 1</t>
+  </si>
+  <si>
+    <t>Prerequisite required.
+Also it is not from the correct school. Reject is Window 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Students already completed this course </t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1339,12 +1436,27 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1402,6 +1514,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1444,21 +1559,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1819,139 +1920,139 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="42">
+      <c r="B3" s="47">
         <v>1</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="51" t="s">
+      <c r="F3" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="52" t="s">
+      <c r="G3" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="38" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="43"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="33"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="37"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="43"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="34" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="43"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="33"/>
+      <c r="B6" s="48"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="37"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="43"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="34" t="s">
+      <c r="B7" s="48"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="34" t="s">
+      <c r="H7" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="I7" s="37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="43"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="33"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="37"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="34" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="I9" s="33" t="s">
+      <c r="I9" s="37" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="41"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="46"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="36">
+      <c r="B11" s="41">
         <v>7</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="43" t="s">
         <v>121</v>
       </c>
       <c r="F11" s="28" t="s">
@@ -1969,10 +2070,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
       <c r="F12" s="28" t="s">
         <v>125</v>
       </c>
@@ -1988,10 +2089,10 @@
     </row>
     <row r="13" spans="1:9" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
       <c r="F13" s="28" t="s">
         <v>122</v>
       </c>
@@ -2007,10 +2108,10 @@
     </row>
     <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
       <c r="F14" s="28" t="s">
         <v>175</v>
       </c>
@@ -2026,10 +2127,10 @@
     </row>
     <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
       <c r="F15" s="28" t="s">
         <v>176</v>
       </c>
@@ -2045,10 +2146,10 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
       <c r="F16" s="22"/>
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
@@ -2511,6 +2612,13 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="D3:D10"/>
+    <mergeCell ref="E3:E10"/>
+    <mergeCell ref="F9:F10"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
@@ -2518,23 +2626,16 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
     <mergeCell ref="B11:B16"/>
     <mergeCell ref="C11:C16"/>
     <mergeCell ref="D11:D16"/>
     <mergeCell ref="E11:E16"/>
     <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="B3:B10"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="D3:D10"/>
-    <mergeCell ref="E3:E10"/>
-    <mergeCell ref="F9:F10"/>
     <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2858,479 +2959,479 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3825DEE-E71C-496C-9D46-14EE94043E6F}">
   <dimension ref="A2:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:I37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="69"/>
-    <col min="2" max="16384" width="14.5703125" style="68"/>
+    <col min="1" max="1" width="14.5703125" style="33"/>
+    <col min="2" max="16384" width="14.5703125" style="32"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="58" t="s">
         <v>180</v>
       </c>
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="58" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67" t="s">
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
-      <c r="B3" s="68" t="s">
+      <c r="A3" s="58"/>
+      <c r="B3" s="32" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="32" t="s">
         <v>184</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="32" t="s">
         <v>188</v>
       </c>
-      <c r="I3" s="68" t="s">
+      <c r="I3" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="J3" s="67"/>
+      <c r="J3" s="58"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="69">
+      <c r="A4" s="33">
         <v>1</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="G4" s="68" t="s">
+      <c r="G4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="H4" s="68" t="s">
+      <c r="H4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="I4" s="68" t="s">
+      <c r="I4" s="32" t="s">
         <v>212</v>
       </c>
-      <c r="J4" s="69"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="120" x14ac:dyDescent="0.25">
-      <c r="A5" s="69">
+      <c r="A5" s="33">
         <v>2</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="32" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="69">
+      <c r="A6" s="33">
         <v>3</v>
       </c>
-      <c r="E6" s="68" t="s">
+      <c r="E6" s="32" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="69">
+      <c r="A7" s="33">
         <v>4</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="F7" s="32" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="69">
+      <c r="A8" s="33">
         <v>5</v>
       </c>
-      <c r="I8" s="68" t="s">
+      <c r="I8" s="32" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="69">
+      <c r="A9" s="33">
         <v>6</v>
       </c>
-      <c r="F9" s="68" t="s">
+      <c r="F9" s="32" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="69">
+      <c r="A10" s="33">
         <v>7</v>
       </c>
-      <c r="G10" s="68" t="s">
+      <c r="G10" s="32" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="69">
+      <c r="A11" s="33">
         <v>8</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="32" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="69">
+      <c r="A12" s="33">
         <v>9</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="32" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="69">
+      <c r="A13" s="33">
         <v>10</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="32" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="69">
+      <c r="A14" s="33">
         <v>11</v>
       </c>
-      <c r="H14" s="68" t="s">
+      <c r="H14" s="32" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="70">
+      <c r="A15" s="34">
         <v>12</v>
       </c>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="69">
+      <c r="A16" s="33">
         <v>13</v>
       </c>
-      <c r="I16" s="68" t="s">
+      <c r="I16" s="32" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="70">
+      <c r="A17" s="34">
         <v>14</v>
       </c>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
     </row>
     <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="69">
+      <c r="A18" s="33">
         <v>15</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="32" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="69">
+      <c r="A19" s="33">
         <v>16</v>
       </c>
-      <c r="C19" s="68" t="s">
+      <c r="C19" s="32" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="69">
+      <c r="A20" s="33">
         <v>17</v>
       </c>
-      <c r="E20" s="68" t="s">
+      <c r="E20" s="32" t="s">
         <v>213</v>
       </c>
-      <c r="F20" s="68" t="s">
+      <c r="F20" s="32" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="70">
+      <c r="A21" s="34">
         <v>18</v>
       </c>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="69">
+      <c r="A22" s="33">
         <v>19</v>
       </c>
-      <c r="G22" s="68" t="s">
+      <c r="G22" s="32" t="s">
         <v>202</v>
       </c>
-      <c r="I22" s="68" t="s">
+      <c r="I22" s="32" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="69">
+      <c r="A23" s="33">
         <v>20</v>
       </c>
-      <c r="B23" s="68" t="s">
+      <c r="B23" s="32" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="70">
+      <c r="A24" s="34">
         <v>21</v>
       </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="71"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="71"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="70">
+      <c r="A25" s="34">
         <v>22</v>
       </c>
-      <c r="B25" s="71"/>
-      <c r="C25" s="71"/>
-      <c r="D25" s="71"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="71"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="71"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
     </row>
     <row r="26" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="69">
+      <c r="A26" s="33">
         <v>23</v>
       </c>
-      <c r="H26" s="68" t="s">
+      <c r="H26" s="32" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="69">
+      <c r="A27" s="33">
         <v>24</v>
       </c>
-      <c r="G27" s="68" t="s">
+      <c r="G27" s="32" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="70">
+      <c r="A28" s="34">
         <v>25</v>
       </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="71"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="71"/>
-      <c r="G28" s="71"/>
-      <c r="H28" s="71"/>
-      <c r="I28" s="71"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="69">
+      <c r="A29" s="33">
         <v>26</v>
       </c>
-      <c r="C29" s="68" t="s">
+      <c r="C29" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="D29" s="68" t="s">
+      <c r="D29" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="E29" s="68" t="s">
+      <c r="E29" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="F29" s="68" t="s">
+      <c r="F29" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="G29" s="68" t="s">
+      <c r="G29" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="H29" s="68" t="s">
+      <c r="H29" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="I29" s="68" t="s">
+      <c r="I29" s="32" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="70">
+      <c r="A30" s="34">
         <v>27</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="71"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="71"/>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="70">
+      <c r="A31" s="34">
         <v>28</v>
       </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="71"/>
-      <c r="G31" s="71"/>
-      <c r="H31" s="71"/>
-      <c r="I31" s="71"/>
+      <c r="B31" s="35"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="69">
+      <c r="A32" s="33">
         <v>29</v>
       </c>
-      <c r="F32" s="68" t="s">
+      <c r="F32" s="32" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="69">
+      <c r="A33" s="33">
         <v>30</v>
       </c>
-      <c r="D33" s="68" t="s">
+      <c r="D33" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="E33" s="68" t="s">
+      <c r="E33" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="F33" s="68" t="s">
+      <c r="F33" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="G33" s="68" t="s">
+      <c r="G33" s="32" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="69">
+      <c r="A34" s="33">
         <v>31</v>
       </c>
-      <c r="D34" s="68" t="s">
+      <c r="D34" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="E34" s="68" t="s">
+      <c r="E34" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="F34" s="68" t="s">
+      <c r="F34" s="32" t="s">
         <v>210</v>
       </c>
-      <c r="G34" s="68" t="s">
+      <c r="G34" s="32" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="70">
+      <c r="A35" s="34">
         <v>32</v>
       </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="71"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="71"/>
-      <c r="H35" s="71"/>
-      <c r="I35" s="71"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
     </row>
     <row r="36" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A36" s="69">
+      <c r="A36" s="33">
         <v>33</v>
       </c>
-      <c r="C36" s="68" t="s">
+      <c r="C36" s="32" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="70">
+      <c r="A37" s="34">
         <v>34</v>
       </c>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="71"/>
-      <c r="F37" s="71"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="71"/>
-      <c r="I37" s="71"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
+      <c r="F37" s="35"/>
+      <c r="G37" s="35"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
     </row>
     <row r="38" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="69">
+      <c r="A38" s="33">
         <v>35</v>
       </c>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="E38" s="68" t="s">
+      <c r="E38" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="F38" s="68" t="s">
+      <c r="F38" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="G38" s="68" t="s">
+      <c r="G38" s="32" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="69">
+      <c r="A39" s="33">
         <v>36</v>
       </c>
-      <c r="D39" s="68" t="s">
+      <c r="D39" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="E39" s="68" t="s">
+      <c r="E39" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="F39" s="68" t="s">
+      <c r="F39" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="G39" s="68" t="s">
+      <c r="G39" s="32" t="s">
         <v>209</v>
       </c>
     </row>
@@ -3345,6 +3446,738 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00A9CBB-888D-4830-9F17-170B0FBAED42}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="15" style="32"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="58"/>
+      <c r="B2" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>218</v>
+      </c>
+      <c r="G2" s="58"/>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="32">
+        <v>2</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="32">
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="32">
+        <v>5</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="32">
+        <v>6</v>
+      </c>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="32">
+        <v>7</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="32">
+        <v>8</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="32">
+        <v>9</v>
+      </c>
+      <c r="E10" s="32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="32">
+        <v>10</v>
+      </c>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="32">
+        <v>11</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="E12" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="32">
+        <v>12</v>
+      </c>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="32">
+        <v>13</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="32">
+        <v>14</v>
+      </c>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="32">
+        <v>15</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="32">
+        <v>16</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="32">
+        <v>17</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="32">
+        <v>18</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="32">
+        <v>19</v>
+      </c>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="32">
+        <v>20</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="32">
+        <v>21</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="32">
+        <v>22</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="32">
+        <v>23</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="32">
+        <v>24</v>
+      </c>
+      <c r="D25" s="32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="32">
+        <v>25</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="32">
+        <v>26</v>
+      </c>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="32">
+        <v>27</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="32">
+        <v>28</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:G2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B50E14-6952-4B07-8FDA-87AFA776EFDF}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="35" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="58"/>
+      <c r="B2" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="D2" s="58"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98741F3-EDD6-4A25-8E75-7E4C0C78576B}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="11.5703125" style="36"/>
+    <col min="4" max="4" width="14.5703125" style="36" customWidth="1"/>
+    <col min="5" max="16384" width="11.5703125" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="58"/>
+      <c r="B2" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>234</v>
+      </c>
+      <c r="F2" s="58"/>
+    </row>
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
+        <v>2</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
+        <v>4</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" s="36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <v>5</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <v>6</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <v>7</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="36">
+        <v>8</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="36">
+        <v>9</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="36">
+        <v>10</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="36">
+        <v>11</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="36">
+        <v>13</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="36">
+        <v>15</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="36">
+        <v>16</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="36">
+        <v>17</v>
+      </c>
+      <c r="C18" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="D18" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="E18" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="36">
+        <v>19</v>
+      </c>
+      <c r="C20" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="D20" s="36" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="36">
+        <v>20</v>
+      </c>
+      <c r="B21" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
+        <v>21</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A23" s="36">
+        <v>22</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>236</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="36">
+        <v>23</v>
+      </c>
+      <c r="D24" s="36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="36">
+        <v>24</v>
+      </c>
+      <c r="B25" s="36" t="s">
+        <v>235</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="36">
+        <v>25</v>
+      </c>
+      <c r="B26" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="58"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="36">
+        <v>26</v>
+      </c>
+      <c r="B27" s="58" t="s">
+        <v>244</v>
+      </c>
+      <c r="C27" s="58"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5331B76C-43B6-4CD9-94DC-A6FA54967D91}">
   <dimension ref="B1:L56"/>
   <sheetViews>
@@ -3399,746 +4232,746 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="36">
+      <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="62" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="60" t="s">
+      <c r="L3" s="66" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="57"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="60"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
+      <c r="K4" s="60"/>
+      <c r="L4" s="66"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
-      <c r="H5" s="56"/>
-      <c r="I5" s="57"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="60"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="66"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="57"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="60"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
+      <c r="K6" s="60"/>
+      <c r="L6" s="66"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="57"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="60"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="66"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="56"/>
-      <c r="H8" s="56"/>
-      <c r="I8" s="57"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="60"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="66"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="55">
+      <c r="B9" s="61">
         <v>2</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="C9" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="I9" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="62" t="s">
+      <c r="L9" s="68" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="55"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="53"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="62"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="59"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="68"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="55"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="53"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="62"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="59"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="68"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="55"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="59"/>
-      <c r="H12" s="59"/>
-      <c r="I12" s="53"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="62"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="59"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="68"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="55"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="59"/>
-      <c r="H13" s="59"/>
-      <c r="I13" s="53"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="62"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="59"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="68"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="55"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="59"/>
-      <c r="H14" s="59"/>
-      <c r="I14" s="53"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="62"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="59"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="68"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="55">
+      <c r="B15" s="61">
         <v>3</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="64" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="59" t="s">
+      <c r="D15" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="55" t="s">
+      <c r="E15" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="55" t="s">
+      <c r="F15" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="55" t="s">
+      <c r="G15" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="55" t="s">
+      <c r="H15" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="53" t="s">
+      <c r="I15" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="54"/>
+      <c r="K15" s="60"/>
       <c r="L15" s="15"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="55"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="53"/>
-      <c r="K16" s="54"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="61"/>
+      <c r="I16" s="59"/>
+      <c r="K16" s="60"/>
       <c r="L16" s="15"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="55"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="53"/>
-      <c r="K17" s="54"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="61"/>
+      <c r="H17" s="61"/>
+      <c r="I17" s="59"/>
+      <c r="K17" s="60"/>
       <c r="L17" s="15"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="55"/>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="53"/>
-      <c r="K18" s="54"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="64"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="59"/>
+      <c r="K18" s="60"/>
       <c r="L18" s="15"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="55"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="53"/>
-      <c r="K19" s="54"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="59"/>
+      <c r="K19" s="60"/>
       <c r="L19" s="15"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="55"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="53"/>
-      <c r="K20" s="54"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="59"/>
+      <c r="K20" s="60"/>
       <c r="L20" s="15"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="55">
+      <c r="B21" s="61">
         <v>4</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="55" t="s">
+      <c r="E21" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="F21" s="55" t="s">
+      <c r="F21" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="55" t="s">
+      <c r="G21" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="55" t="s">
+      <c r="H21" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="53" t="s">
+      <c r="I21" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="K21" s="54"/>
+      <c r="K21" s="60"/>
       <c r="L21" s="15"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="55"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="53"/>
-      <c r="K22" s="54"/>
+      <c r="B22" s="61"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="59"/>
+      <c r="K22" s="60"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="55"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="53"/>
-      <c r="K23" s="54"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="64"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="59"/>
+      <c r="K23" s="60"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="55"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="53"/>
-      <c r="K24" s="54"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="59"/>
+      <c r="K24" s="60"/>
       <c r="L24" s="15"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="55"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="55"/>
-      <c r="F25" s="55"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="55"/>
-      <c r="I25" s="53"/>
-      <c r="K25" s="54"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="59"/>
+      <c r="K25" s="60"/>
       <c r="L25" s="15"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="55"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="59"/>
-      <c r="E26" s="55"/>
-      <c r="F26" s="55"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="55"/>
-      <c r="I26" s="53"/>
-      <c r="K26" s="54"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="64"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="59"/>
+      <c r="K26" s="60"/>
       <c r="L26" s="15"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="55">
+      <c r="B27" s="61">
         <v>5</v>
       </c>
-      <c r="C27" s="58">
+      <c r="C27" s="64">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D27" s="59" t="s">
+      <c r="D27" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="59" t="s">
+      <c r="E27" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="59" t="s">
+      <c r="F27" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="59" t="s">
+      <c r="G27" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="59" t="s">
+      <c r="H27" s="65" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="53" t="s">
+      <c r="I27" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="K27" s="61" t="s">
+      <c r="K27" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="L27" s="60"/>
+      <c r="L27" s="66"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="55"/>
-      <c r="C28" s="58"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="53"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="60"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="64"/>
+      <c r="D28" s="65"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="59"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="66"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="55"/>
-      <c r="C29" s="58"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="53"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="60"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="64"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="59"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="66"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="55"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="59"/>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="59"/>
-      <c r="H30" s="59"/>
-      <c r="I30" s="53"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="60"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="65"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="59"/>
+      <c r="K30" s="67"/>
+      <c r="L30" s="66"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="55"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="59"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="53"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="60"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="59"/>
+      <c r="K31" s="67"/>
+      <c r="L31" s="66"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="55"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="59"/>
-      <c r="E32" s="59"/>
-      <c r="F32" s="59"/>
-      <c r="G32" s="59"/>
-      <c r="H32" s="59"/>
-      <c r="I32" s="53"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="60"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="59"/>
+      <c r="K32" s="67"/>
+      <c r="L32" s="66"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="55">
+      <c r="B33" s="61">
         <v>6</v>
       </c>
-      <c r="C33" s="58" t="s">
+      <c r="C33" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="59" t="s">
+      <c r="D33" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="59" t="s">
+      <c r="E33" s="65" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="59" t="s">
+      <c r="F33" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="59" t="s">
+      <c r="G33" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="55" t="s">
+      <c r="H33" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="I33" s="53" t="s">
+      <c r="I33" s="59" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="55"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="53"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="59"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="55"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="59"/>
-      <c r="E35" s="59"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="53"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="59"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="55"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="59"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="53"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="59"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="55"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="53"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="59"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B38" s="55"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="55"/>
-      <c r="I38" s="53"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="59"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B39" s="55">
+      <c r="B39" s="61">
         <v>7</v>
       </c>
-      <c r="C39" s="58" t="s">
+      <c r="C39" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="65" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="59" t="s">
+      <c r="E39" s="65" t="s">
         <v>104</v>
       </c>
-      <c r="F39" s="59" t="s">
+      <c r="F39" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="G39" s="59" t="s">
+      <c r="G39" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="H39" s="59" t="s">
+      <c r="H39" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="I39" s="53" t="s">
+      <c r="I39" s="59" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="55"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="59"/>
-      <c r="E40" s="59"/>
-      <c r="F40" s="59"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="59"/>
-      <c r="I40" s="53"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
+      <c r="E40" s="65"/>
+      <c r="F40" s="65"/>
+      <c r="G40" s="65"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="59"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B41" s="55"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="59"/>
-      <c r="H41" s="59"/>
-      <c r="I41" s="53"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="64"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="59"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B42" s="55"/>
-      <c r="C42" s="58"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="59"/>
-      <c r="I42" s="53"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="64"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="59"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="55"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="59"/>
-      <c r="E43" s="59"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="53"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="59"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="55"/>
-      <c r="C44" s="58"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="59"/>
-      <c r="F44" s="59"/>
-      <c r="G44" s="59"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="53"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="64"/>
+      <c r="D44" s="65"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="65"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="59"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="55">
+      <c r="B45" s="61">
         <v>8</v>
       </c>
-      <c r="C45" s="58" t="s">
+      <c r="C45" s="64" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="59" t="s">
+      <c r="D45" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="E45" s="59" t="s">
+      <c r="E45" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="F45" s="59" t="s">
+      <c r="F45" s="65" t="s">
         <v>112</v>
       </c>
-      <c r="G45" s="63" t="s">
+      <c r="G45" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="55" t="s">
+      <c r="H45" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="I45" s="55" t="s">
+      <c r="I45" s="61" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="55"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59"/>
-      <c r="F46" s="59"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="64"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B47" s="55"/>
-      <c r="C47" s="58"/>
-      <c r="D47" s="59"/>
-      <c r="E47" s="59"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="65"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B48" s="55"/>
-      <c r="C48" s="58"/>
-      <c r="D48" s="59"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="59"/>
-      <c r="G48" s="63"/>
-      <c r="H48" s="55"/>
-      <c r="I48" s="55"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="65"/>
+      <c r="E48" s="65"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="69"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="55"/>
-      <c r="C49" s="58"/>
-      <c r="D49" s="59"/>
-      <c r="E49" s="59"/>
-      <c r="F49" s="59"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="55"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="65"/>
+      <c r="E49" s="65"/>
+      <c r="F49" s="65"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B50" s="55"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="59"/>
-      <c r="E50" s="59"/>
-      <c r="F50" s="59"/>
-      <c r="G50" s="63"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="55"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="65"/>
+      <c r="G50" s="69"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="65">
+      <c r="B51" s="71">
         <v>8</v>
       </c>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="64"/>
-      <c r="E51" s="64"/>
-      <c r="F51" s="64"/>
-      <c r="G51" s="64"/>
-      <c r="H51" s="64"/>
-      <c r="I51" s="64"/>
+      <c r="D51" s="70"/>
+      <c r="E51" s="70"/>
+      <c r="F51" s="70"/>
+      <c r="G51" s="70"/>
+      <c r="H51" s="70"/>
+      <c r="I51" s="70"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B52" s="65"/>
-      <c r="C52" s="66"/>
-      <c r="D52" s="64"/>
-      <c r="E52" s="64"/>
-      <c r="F52" s="64"/>
-      <c r="G52" s="64"/>
-      <c r="H52" s="64"/>
-      <c r="I52" s="64"/>
+      <c r="B52" s="71"/>
+      <c r="C52" s="72"/>
+      <c r="D52" s="70"/>
+      <c r="E52" s="70"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+      <c r="I52" s="70"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B53" s="65"/>
-      <c r="C53" s="66"/>
-      <c r="D53" s="64"/>
-      <c r="E53" s="64"/>
-      <c r="F53" s="64"/>
-      <c r="G53" s="64"/>
-      <c r="H53" s="64"/>
-      <c r="I53" s="64"/>
+      <c r="B53" s="71"/>
+      <c r="C53" s="72"/>
+      <c r="D53" s="70"/>
+      <c r="E53" s="70"/>
+      <c r="F53" s="70"/>
+      <c r="G53" s="70"/>
+      <c r="H53" s="70"/>
+      <c r="I53" s="70"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B54" s="65"/>
-      <c r="C54" s="66"/>
-      <c r="D54" s="64"/>
-      <c r="E54" s="64"/>
-      <c r="F54" s="64"/>
-      <c r="G54" s="64"/>
-      <c r="H54" s="64"/>
-      <c r="I54" s="64"/>
+      <c r="B54" s="71"/>
+      <c r="C54" s="72"/>
+      <c r="D54" s="70"/>
+      <c r="E54" s="70"/>
+      <c r="F54" s="70"/>
+      <c r="G54" s="70"/>
+      <c r="H54" s="70"/>
+      <c r="I54" s="70"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B55" s="65"/>
-      <c r="C55" s="66"/>
-      <c r="D55" s="64"/>
-      <c r="E55" s="64"/>
-      <c r="F55" s="64"/>
-      <c r="G55" s="64"/>
-      <c r="H55" s="64"/>
-      <c r="I55" s="64"/>
+      <c r="B55" s="71"/>
+      <c r="C55" s="72"/>
+      <c r="D55" s="70"/>
+      <c r="E55" s="70"/>
+      <c r="F55" s="70"/>
+      <c r="G55" s="70"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B56" s="65"/>
-      <c r="C56" s="66"/>
-      <c r="D56" s="64"/>
-      <c r="E56" s="64"/>
-      <c r="F56" s="64"/>
-      <c r="G56" s="64"/>
-      <c r="H56" s="64"/>
-      <c r="I56" s="64"/>
+      <c r="B56" s="71"/>
+      <c r="C56" s="72"/>
+      <c r="D56" s="70"/>
+      <c r="E56" s="70"/>
+      <c r="F56" s="70"/>
+      <c r="G56" s="70"/>
+      <c r="H56" s="70"/>
+      <c r="I56" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="80">
@@ -4228,15 +5061,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE41C69-7513-44E6-A818-D455BC48C7D6}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
   <dimension ref="A2:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Bug Metric and Testcases
Co-Authored-By: simshengqin <simshengqin@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Testing/Testcases.xlsx
+++ b/Testing/Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\project-g4t6\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AC88651-CA32-44CE-A224-C33B0E13A415}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73C0818-0441-4984-94F7-22FFA8D14449}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{E90EB661-BF25-40DF-8004-68D825EA22BE}"/>
   </bookViews>
@@ -1859,15 +1859,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1904,23 +1925,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1930,45 +1969,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2287,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A4A64FB-D5C5-440E-AB26-01D6449FC916}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2330,139 +2330,139 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39">
+      <c r="B3" s="46">
         <v>1</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="49" t="s">
+      <c r="G3" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="49" t="s">
+      <c r="H3" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="37" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="40"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="37"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="40"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="35" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="G5" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="38" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="40"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="37"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="38"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="40"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="35" t="s">
+      <c r="B7" s="47"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="G7" s="50" t="s">
+      <c r="G7" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="I7" s="37" t="s">
+      <c r="I7" s="38" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="40"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="37"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="38"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="35" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="G9" s="50" t="s">
+      <c r="G9" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="39" t="s">
         <v>128</v>
       </c>
-      <c r="I9" s="37" t="s">
+      <c r="I9" s="38" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="38"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="51"/>
+      <c r="D10" s="54"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="43"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="51">
+      <c r="B11" s="41">
         <v>7</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="69" t="s">
+      <c r="E11" s="42" t="s">
         <v>121</v>
       </c>
       <c r="F11" s="22" t="s">
@@ -2480,10 +2480,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
       <c r="F12" s="22" t="s">
         <v>125</v>
       </c>
@@ -2499,10 +2499,10 @@
     </row>
     <row r="13" spans="1:9" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="22" t="s">
         <v>122</v>
       </c>
@@ -2518,10 +2518,10 @@
     </row>
     <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="22" t="s">
         <v>196</v>
       </c>
@@ -2537,10 +2537,10 @@
     </row>
     <row r="15" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="22" t="s">
         <v>197</v>
       </c>
@@ -2556,10 +2556,10 @@
     </row>
     <row r="16" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
       <c r="F16" s="32" t="s">
         <v>199</v>
       </c>
@@ -2575,10 +2575,10 @@
     </row>
     <row r="17" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="32" t="s">
         <v>201</v>
       </c>
@@ -2594,10 +2594,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
       <c r="F18" s="32" t="s">
         <v>203</v>
       </c>
@@ -2613,10 +2613,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="42"/>
       <c r="F19" s="32" t="s">
         <v>204</v>
       </c>
@@ -2632,10 +2632,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="42"/>
+      <c r="E20" s="42"/>
       <c r="F20" s="32" t="s">
         <v>205</v>
       </c>
@@ -2651,10 +2651,10 @@
     </row>
     <row r="21" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
       <c r="F21" s="32" t="s">
         <v>206</v>
       </c>
@@ -2670,10 +2670,10 @@
     </row>
     <row r="22" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="32" t="s">
         <v>207</v>
       </c>
@@ -2689,10 +2689,10 @@
     </row>
     <row r="23" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="32" t="s">
         <v>208</v>
       </c>
@@ -2708,10 +2708,10 @@
     </row>
     <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
       <c r="F24" s="32" t="s">
         <v>209</v>
       </c>
@@ -2727,10 +2727,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="32" t="s">
         <v>210</v>
       </c>
@@ -2746,10 +2746,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="32" t="s">
         <v>211</v>
       </c>
@@ -2765,10 +2765,10 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
-      <c r="B27" s="51"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
       <c r="F27" s="32" t="s">
         <v>212</v>
       </c>
@@ -2784,10 +2784,10 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="32" t="s">
         <v>213</v>
       </c>
@@ -2803,10 +2803,10 @@
     </row>
     <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="32" t="s">
         <v>214</v>
       </c>
@@ -2822,10 +2822,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="42"/>
+      <c r="E30" s="42"/>
       <c r="F30" s="32" t="s">
         <v>216</v>
       </c>
@@ -2841,10 +2841,10 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="41"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
       <c r="F31" s="32" t="s">
         <v>217</v>
       </c>
@@ -2860,10 +2860,10 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="41"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="42"/>
       <c r="F32" s="32" t="s">
         <v>218</v>
       </c>
@@ -2879,10 +2879,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
-      <c r="B33" s="51"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
+      <c r="B33" s="41"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
       <c r="F33" s="32" t="s">
         <v>219</v>
       </c>
@@ -2898,10 +2898,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="69"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="42"/>
+      <c r="E34" s="42"/>
       <c r="F34" s="32" t="s">
         <v>220</v>
       </c>
@@ -2911,7 +2911,7 @@
       <c r="H34" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="I34" s="70" t="s">
+      <c r="I34" s="35" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3209,6 +3209,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="I3:I4"/>
     <mergeCell ref="F5:F6"/>
     <mergeCell ref="G5:G6"/>
@@ -3225,14 +3233,6 @@
     <mergeCell ref="E3:E10"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3256,150 +3256,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="71"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="71"/>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="71"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="71"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="71"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="71"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="71"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="71"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="71"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="71"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="71"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
-      <c r="D13" s="71"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="71"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="71"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
-      <c r="D15" s="71"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="71"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="71"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
       <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="71"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
-      <c r="B19" s="71"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
       <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="71"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="71"/>
-      <c r="D20" s="71"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
       <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="71"/>
-      <c r="B21" s="71"/>
-      <c r="C21" s="71"/>
-      <c r="D21" s="71"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
       <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -3436,25 +3436,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55" t="s">
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="55"/>
+      <c r="A3" s="57"/>
       <c r="B3" s="26" t="s">
         <v>132</v>
       </c>
@@ -3479,7 +3479,7 @@
       <c r="I3" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="J3" s="55"/>
+      <c r="J3" s="57"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="27">
@@ -3925,22 +3925,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="26" t="s">
         <v>164</v>
       </c>
@@ -3956,7 +3956,7 @@
       <c r="F2" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="G2" s="55"/>
+      <c r="G2" s="57"/>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="26">
@@ -4238,14 +4238,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57" t="s">
         <v>76</v>
       </c>
       <c r="E1" s="26"/>
@@ -4253,14 +4253,14 @@
       <c r="G1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="26" t="s">
         <v>132</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>179</v>
       </c>
-      <c r="D2" s="55"/>
+      <c r="D2" s="57"/>
       <c r="E2" s="26"/>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
@@ -4360,21 +4360,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="57" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55" t="s">
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="55"/>
+      <c r="A2" s="57"/>
       <c r="B2" s="30" t="s">
         <v>164</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="E2" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="F2" s="55"/>
+      <c r="F2" s="57"/>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="30">
@@ -4613,23 +4613,23 @@
       <c r="A26" s="30">
         <v>25</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="C26" s="57"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="30">
         <v>26</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="C27" s="55"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="55"/>
+      <c r="C27" s="57"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4698,123 +4698,123 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B3" s="51">
+      <c r="B3" s="41">
         <v>1</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="68" t="s">
+      <c r="E3" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="68" t="s">
+      <c r="F3" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="68" t="s">
+      <c r="H3" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="69" t="s">
+      <c r="I3" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="K3" s="64" t="s">
+      <c r="K3" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="66" t="s">
+      <c r="L3" s="65" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B4" s="51"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="69"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="66"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="42"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="65"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="69"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="66"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="42"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="65"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B6" s="51"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="69"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="66"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="61"/>
+      <c r="I6" s="42"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="65"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B7" s="51"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="68"/>
-      <c r="H7" s="68"/>
-      <c r="I7" s="69"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="66"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="42"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="65"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B8" s="51"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="69"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="66"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="42"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="65"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B9" s="62">
+      <c r="B9" s="60">
         <v>2</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="60" t="s">
+      <c r="H9" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="K9" s="64" t="s">
+      <c r="K9" s="59" t="s">
         <v>84</v>
       </c>
       <c r="L9" s="67" t="s">
@@ -4822,632 +4822,682 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B10" s="62"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="59"/>
-      <c r="K10" s="64"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="63"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="58"/>
+      <c r="K10" s="59"/>
       <c r="L10" s="67"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B11" s="62"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="59"/>
-      <c r="K11" s="64"/>
+      <c r="B11" s="60"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="63"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="58"/>
+      <c r="K11" s="59"/>
       <c r="L11" s="67"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B12" s="62"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="60"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="59"/>
-      <c r="K12" s="64"/>
+      <c r="B12" s="60"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="58"/>
+      <c r="K12" s="59"/>
       <c r="L12" s="67"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B13" s="62"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="59"/>
-      <c r="K13" s="64"/>
+      <c r="B13" s="60"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="58"/>
+      <c r="K13" s="59"/>
       <c r="L13" s="67"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B14" s="62"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="59"/>
-      <c r="K14" s="64"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="58"/>
+      <c r="K14" s="59"/>
       <c r="L14" s="67"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B15" s="62">
+      <c r="B15" s="60">
         <v>3</v>
       </c>
-      <c r="C15" s="63" t="s">
+      <c r="C15" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="62" t="s">
+      <c r="E15" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="F15" s="62" t="s">
+      <c r="F15" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="G15" s="62" t="s">
+      <c r="G15" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="H15" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="59" t="s">
+      <c r="I15" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="64"/>
+      <c r="K15" s="59"/>
       <c r="L15" s="15"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B16" s="62"/>
-      <c r="C16" s="63"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="59"/>
-      <c r="K16" s="64"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="63"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="58"/>
+      <c r="K16" s="59"/>
       <c r="L16" s="15"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B17" s="62"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="59"/>
-      <c r="K17" s="64"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="58"/>
+      <c r="K17" s="59"/>
       <c r="L17" s="15"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B18" s="62"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="59"/>
-      <c r="K18" s="64"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="63"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="58"/>
+      <c r="K18" s="59"/>
       <c r="L18" s="15"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B19" s="62"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="59"/>
-      <c r="K19" s="64"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="58"/>
+      <c r="K19" s="59"/>
       <c r="L19" s="15"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B20" s="62"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="59"/>
-      <c r="K20" s="64"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="60"/>
+      <c r="I20" s="58"/>
+      <c r="K20" s="59"/>
       <c r="L20" s="15"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B21" s="62">
+      <c r="B21" s="60">
         <v>4</v>
       </c>
-      <c r="C21" s="63" t="s">
+      <c r="C21" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="D21" s="60" t="s">
+      <c r="D21" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="E21" s="62" t="s">
+      <c r="E21" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="F21" s="62" t="s">
+      <c r="F21" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="G21" s="62" t="s">
+      <c r="G21" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="H21" s="62" t="s">
+      <c r="H21" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="I21" s="59" t="s">
+      <c r="I21" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="K21" s="64"/>
+      <c r="K21" s="59"/>
       <c r="L21" s="15"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B22" s="62"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="59"/>
-      <c r="K22" s="64"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="60"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="60"/>
+      <c r="I22" s="58"/>
+      <c r="K22" s="59"/>
       <c r="L22" s="15"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B23" s="62"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="59"/>
-      <c r="K23" s="64"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="58"/>
+      <c r="K23" s="59"/>
       <c r="L23" s="15"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B24" s="62"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="59"/>
-      <c r="K24" s="64"/>
+      <c r="B24" s="60"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="60"/>
+      <c r="F24" s="60"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="60"/>
+      <c r="I24" s="58"/>
+      <c r="K24" s="59"/>
       <c r="L24" s="15"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B25" s="62"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="59"/>
-      <c r="K25" s="64"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="58"/>
+      <c r="K25" s="59"/>
       <c r="L25" s="15"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B26" s="62"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="59"/>
-      <c r="K26" s="64"/>
+      <c r="B26" s="60"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="60"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="58"/>
+      <c r="K26" s="59"/>
       <c r="L26" s="15"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B27" s="62">
+      <c r="B27" s="60">
         <v>5</v>
       </c>
-      <c r="C27" s="63">
+      <c r="C27" s="62">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D27" s="60" t="s">
+      <c r="D27" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="60" t="s">
+      <c r="E27" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="F27" s="60" t="s">
+      <c r="F27" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="60" t="s">
+      <c r="G27" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="H27" s="60" t="s">
+      <c r="H27" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="59" t="s">
+      <c r="I27" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="K27" s="65" t="s">
+      <c r="K27" s="66" t="s">
         <v>74</v>
       </c>
-      <c r="L27" s="66"/>
+      <c r="L27" s="65"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B28" s="62"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="60"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="59"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="66"/>
+      <c r="B28" s="60"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="63"/>
+      <c r="G28" s="63"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="58"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="65"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B29" s="62"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="59"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="66"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
+      <c r="I29" s="58"/>
+      <c r="K29" s="66"/>
+      <c r="L29" s="65"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B30" s="62"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="59"/>
-      <c r="K30" s="65"/>
-      <c r="L30" s="66"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="58"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="65"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B31" s="62"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="59"/>
-      <c r="K31" s="65"/>
-      <c r="L31" s="66"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="63"/>
+      <c r="I31" s="58"/>
+      <c r="K31" s="66"/>
+      <c r="L31" s="65"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B32" s="62"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="60"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="59"/>
-      <c r="K32" s="65"/>
-      <c r="L32" s="66"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="I32" s="58"/>
+      <c r="K32" s="66"/>
+      <c r="L32" s="65"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="62">
+      <c r="B33" s="60">
         <v>6</v>
       </c>
-      <c r="C33" s="63" t="s">
+      <c r="C33" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="D33" s="60" t="s">
+      <c r="D33" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="60" t="s">
+      <c r="E33" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="60" t="s">
+      <c r="F33" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="60" t="s">
+      <c r="G33" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="H33" s="62" t="s">
+      <c r="H33" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="I33" s="59" t="s">
+      <c r="I33" s="58" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="62"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="60"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="59"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
+      <c r="G34" s="63"/>
+      <c r="H34" s="60"/>
+      <c r="I34" s="58"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="62"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="59"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="62"/>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="58"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="62"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
-      <c r="F36" s="60"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="59"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="62"/>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+      <c r="F36" s="63"/>
+      <c r="G36" s="63"/>
+      <c r="H36" s="60"/>
+      <c r="I36" s="58"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="62"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
-      <c r="G37" s="60"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="59"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="62"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="60"/>
+      <c r="I37" s="58"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="62"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="62"/>
-      <c r="I38" s="59"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
+      <c r="F38" s="63"/>
+      <c r="G38" s="63"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="58"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="62">
+      <c r="B39" s="60">
         <v>7</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="E39" s="60" t="s">
+      <c r="E39" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="F39" s="60" t="s">
+      <c r="F39" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="G39" s="60" t="s">
+      <c r="G39" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="H39" s="60" t="s">
+      <c r="H39" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="I39" s="59" t="s">
+      <c r="I39" s="58" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="62"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="60"/>
-      <c r="G40" s="60"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="59"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="63"/>
+      <c r="H40" s="63"/>
+      <c r="I40" s="58"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="62"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="60"/>
-      <c r="G41" s="60"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="59"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="58"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="62"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="60"/>
-      <c r="G42" s="60"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="59"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="63"/>
+      <c r="H42" s="63"/>
+      <c r="I42" s="58"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="62"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
-      <c r="H43" s="60"/>
-      <c r="I43" s="59"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="63"/>
+      <c r="H43" s="63"/>
+      <c r="I43" s="58"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="62"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="60"/>
-      <c r="G44" s="60"/>
-      <c r="H44" s="60"/>
-      <c r="I44" s="59"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="63"/>
+      <c r="H44" s="63"/>
+      <c r="I44" s="58"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B45" s="62">
+      <c r="B45" s="60">
         <v>8</v>
       </c>
-      <c r="C45" s="63" t="s">
+      <c r="C45" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="D45" s="60" t="s">
+      <c r="D45" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="E45" s="60" t="s">
+      <c r="E45" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="F45" s="60" t="s">
+      <c r="F45" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="G45" s="61" t="s">
+      <c r="G45" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="H45" s="62" t="s">
+      <c r="H45" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="I45" s="62" t="s">
+      <c r="I45" s="60" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B46" s="62"/>
-      <c r="C46" s="63"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="60"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="62"/>
-      <c r="I46" s="62"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="60"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B47" s="62"/>
-      <c r="C47" s="63"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
-      <c r="F47" s="60"/>
-      <c r="G47" s="61"/>
-      <c r="H47" s="62"/>
-      <c r="I47" s="62"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
+      <c r="F47" s="63"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B48" s="62"/>
-      <c r="C48" s="63"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
-      <c r="F48" s="60"/>
-      <c r="G48" s="61"/>
-      <c r="H48" s="62"/>
-      <c r="I48" s="62"/>
+      <c r="B48" s="60"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
+      <c r="F48" s="63"/>
+      <c r="G48" s="68"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B49" s="62"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
-      <c r="F49" s="60"/>
-      <c r="G49" s="61"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="62"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="68"/>
+      <c r="H49" s="60"/>
+      <c r="I49" s="60"/>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B50" s="62"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
-      <c r="F50" s="60"/>
-      <c r="G50" s="61"/>
-      <c r="H50" s="62"/>
-      <c r="I50" s="62"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="68"/>
+      <c r="H50" s="60"/>
+      <c r="I50" s="60"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B51" s="57">
+      <c r="B51" s="70">
         <v>8</v>
       </c>
-      <c r="C51" s="58" t="s">
+      <c r="C51" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="56"/>
-      <c r="H51" s="56"/>
-      <c r="I51" s="56"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69"/>
+      <c r="H51" s="69"/>
+      <c r="I51" s="69"/>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B52" s="57"/>
-      <c r="C52" s="58"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="56"/>
-      <c r="H52" s="56"/>
-      <c r="I52" s="56"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="71"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="69"/>
+      <c r="I52" s="69"/>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="57"/>
-      <c r="C53" s="58"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="56"/>
-      <c r="H53" s="56"/>
-      <c r="I53" s="56"/>
+      <c r="B53" s="70"/>
+      <c r="C53" s="71"/>
+      <c r="D53" s="69"/>
+      <c r="E53" s="69"/>
+      <c r="F53" s="69"/>
+      <c r="G53" s="69"/>
+      <c r="H53" s="69"/>
+      <c r="I53" s="69"/>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="57"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="56"/>
-      <c r="H54" s="56"/>
-      <c r="I54" s="56"/>
+      <c r="B54" s="70"/>
+      <c r="C54" s="71"/>
+      <c r="D54" s="69"/>
+      <c r="E54" s="69"/>
+      <c r="F54" s="69"/>
+      <c r="G54" s="69"/>
+      <c r="H54" s="69"/>
+      <c r="I54" s="69"/>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B55" s="57"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="56"/>
-      <c r="H55" s="56"/>
-      <c r="I55" s="56"/>
+      <c r="B55" s="70"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
+      <c r="F55" s="69"/>
+      <c r="G55" s="69"/>
+      <c r="H55" s="69"/>
+      <c r="I55" s="69"/>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B56" s="57"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="56"/>
-      <c r="H56" s="56"/>
-      <c r="I56" s="56"/>
+      <c r="B56" s="70"/>
+      <c r="C56" s="71"/>
+      <c r="D56" s="69"/>
+      <c r="E56" s="69"/>
+      <c r="F56" s="69"/>
+      <c r="G56" s="69"/>
+      <c r="H56" s="69"/>
+      <c r="I56" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="I21:I26"/>
-    <mergeCell ref="K15:K20"/>
-    <mergeCell ref="K21:K26"/>
-    <mergeCell ref="G15:G20"/>
-    <mergeCell ref="H15:H20"/>
-    <mergeCell ref="G21:G26"/>
-    <mergeCell ref="H21:H26"/>
+    <mergeCell ref="G51:G56"/>
+    <mergeCell ref="H51:H56"/>
+    <mergeCell ref="I51:I56"/>
+    <mergeCell ref="B51:B56"/>
+    <mergeCell ref="C51:C56"/>
+    <mergeCell ref="D51:D56"/>
+    <mergeCell ref="E51:E56"/>
+    <mergeCell ref="F51:F56"/>
+    <mergeCell ref="I39:I44"/>
+    <mergeCell ref="D45:D50"/>
+    <mergeCell ref="E45:E50"/>
+    <mergeCell ref="F45:F50"/>
+    <mergeCell ref="G45:G50"/>
+    <mergeCell ref="H45:H50"/>
+    <mergeCell ref="I45:I50"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="C45:C50"/>
+    <mergeCell ref="E39:E44"/>
+    <mergeCell ref="F39:F44"/>
+    <mergeCell ref="D15:D20"/>
+    <mergeCell ref="E15:E20"/>
+    <mergeCell ref="F15:F20"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F26"/>
+    <mergeCell ref="K3:K8"/>
+    <mergeCell ref="K27:K32"/>
+    <mergeCell ref="L3:L8"/>
+    <mergeCell ref="I15:I20"/>
+    <mergeCell ref="B45:B50"/>
+    <mergeCell ref="H9:H14"/>
+    <mergeCell ref="I9:I14"/>
+    <mergeCell ref="K9:K14"/>
+    <mergeCell ref="L9:L14"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="C9:C14"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="E9:E14"/>
+    <mergeCell ref="F9:F14"/>
+    <mergeCell ref="L27:L32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="D27:D32"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="F27:F32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="I27:I32"/>
+    <mergeCell ref="B3:B8"/>
+    <mergeCell ref="C3:C8"/>
+    <mergeCell ref="D3:D8"/>
+    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="F3:F8"/>
     <mergeCell ref="G3:G8"/>
     <mergeCell ref="H3:H8"/>
     <mergeCell ref="I3:I8"/>
@@ -5464,63 +5514,13 @@
     <mergeCell ref="G9:G14"/>
     <mergeCell ref="G39:G44"/>
     <mergeCell ref="H39:H44"/>
-    <mergeCell ref="B3:B8"/>
-    <mergeCell ref="C3:C8"/>
-    <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:E8"/>
-    <mergeCell ref="F3:F8"/>
-    <mergeCell ref="L27:L32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="D27:D32"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="F27:F32"/>
-    <mergeCell ref="H27:H32"/>
-    <mergeCell ref="I27:I32"/>
-    <mergeCell ref="K3:K8"/>
-    <mergeCell ref="K27:K32"/>
-    <mergeCell ref="L3:L8"/>
-    <mergeCell ref="I15:I20"/>
-    <mergeCell ref="B45:B50"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="I9:I14"/>
-    <mergeCell ref="K9:K14"/>
-    <mergeCell ref="L9:L14"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="C9:C14"/>
-    <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E9:E14"/>
-    <mergeCell ref="F9:F14"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="C45:C50"/>
-    <mergeCell ref="E39:E44"/>
-    <mergeCell ref="F39:F44"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="F15:F20"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F26"/>
-    <mergeCell ref="I39:I44"/>
-    <mergeCell ref="D45:D50"/>
-    <mergeCell ref="E45:E50"/>
-    <mergeCell ref="F45:F50"/>
-    <mergeCell ref="G45:G50"/>
-    <mergeCell ref="H45:H50"/>
-    <mergeCell ref="I45:I50"/>
-    <mergeCell ref="G51:G56"/>
-    <mergeCell ref="H51:H56"/>
-    <mergeCell ref="I51:I56"/>
-    <mergeCell ref="B51:B56"/>
-    <mergeCell ref="C51:C56"/>
-    <mergeCell ref="D51:D56"/>
-    <mergeCell ref="E51:E56"/>
-    <mergeCell ref="F51:F56"/>
+    <mergeCell ref="I21:I26"/>
+    <mergeCell ref="K15:K20"/>
+    <mergeCell ref="K21:K26"/>
+    <mergeCell ref="G15:G20"/>
+    <mergeCell ref="H15:H20"/>
+    <mergeCell ref="G21:G26"/>
+    <mergeCell ref="H21:H26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>